<commit_message>
results and pictures updated
</commit_message>
<xml_diff>
--- a/BIDMC/np_swab_results.xlsx
+++ b/BIDMC/np_swab_results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="775">
   <si>
     <t>Date of test</t>
   </si>
@@ -2221,6 +2221,135 @@
   </si>
   <si>
     <t>nylong 12</t>
+  </si>
+  <si>
+    <t>Did not pass. Less sharp</t>
+  </si>
+  <si>
+    <t>pass. sharp</t>
+  </si>
+  <si>
+    <t>Did not pass. Sharp</t>
+  </si>
+  <si>
+    <t>did not test-powder material</t>
+  </si>
+  <si>
+    <t>did not test- residue</t>
+  </si>
+  <si>
+    <t>J_3_1</t>
+  </si>
+  <si>
+    <t>resin 'flock' tip</t>
+  </si>
+  <si>
+    <t>fail-I think, it doesn't bend back to shape, I thinj will have trouble getting to posterior NP. Smells Odd.</t>
+  </si>
+  <si>
+    <t>did not test- smells</t>
+  </si>
+  <si>
+    <t>C_V3_20v9.1</t>
+  </si>
+  <si>
+    <t>carbon swab with z-axis struts</t>
+  </si>
+  <si>
+    <t>pass. Tip seems softer, although other swabs may still be more comfortable</t>
+  </si>
+  <si>
+    <t>C_Hv5_35v9</t>
+  </si>
+  <si>
+    <t>carbon swab with sinusoidal center strut</t>
+  </si>
+  <si>
+    <t>pass. Softer, narrower tip, may still not be favorite but better imo</t>
+  </si>
+  <si>
+    <t>C_V3_15v1</t>
+  </si>
+  <si>
+    <t>carbon swab with short tip</t>
+  </si>
+  <si>
+    <t>pass. Seems [/more]similar to envision or the others &amp; the tip is softer</t>
+  </si>
+  <si>
+    <t>PCTW</t>
+  </si>
+  <si>
+    <t>puritan sterile cotton tipped applicator w/wood handle. ref 25-826 5WC</t>
+  </si>
+  <si>
+    <t>cotton and wood</t>
+  </si>
+  <si>
+    <t>PCT</t>
+  </si>
+  <si>
+    <t>puritan cotton swab with plastic handle. ref 25-806 1PC</t>
+  </si>
+  <si>
+    <t>cotton and plastic</t>
+  </si>
+  <si>
+    <t>FPR</t>
+  </si>
+  <si>
+    <t>fisher polyester-tipped applicators</t>
+  </si>
+  <si>
+    <t>polyester</t>
+  </si>
+  <si>
+    <t>3DS_NP4</t>
+  </si>
+  <si>
+    <t>resin print tip with tight hex mesh</t>
+  </si>
+  <si>
+    <t>resin</t>
+  </si>
+  <si>
+    <t>Patrick Dunne. Patrick.Dunne@3dsystems.com</t>
+  </si>
+  <si>
+    <t>3DS_NP3</t>
+  </si>
+  <si>
+    <t>3DS_NP2</t>
+  </si>
+  <si>
+    <t>resin print tip with tight helical mesh</t>
+  </si>
+  <si>
+    <t>3DS_NP1</t>
+  </si>
+  <si>
+    <t>resin print with tight mesh</t>
+  </si>
+  <si>
+    <t>J_3_2</t>
+  </si>
+  <si>
+    <t>did not test. residue</t>
+  </si>
+  <si>
+    <t>3DPT_LN</t>
+  </si>
+  <si>
+    <t>white swab with large nubbed tip</t>
+  </si>
+  <si>
+    <t>did not test. resiude</t>
+  </si>
+  <si>
+    <t>3DPT_SN</t>
+  </si>
+  <si>
+    <t>white swab with small nubbed tip</t>
   </si>
 </sst>
 </file>
@@ -2699,7 +2828,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2710,10 +2839,10 @@
   <dimension ref="A1:AB1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B174" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B186" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D185" sqref="D185"/>
+      <selection pane="bottomRight" activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -10548,7 +10677,9 @@
         <v>695</v>
       </c>
       <c r="K166" s="8"/>
-      <c r="L166" s="8"/>
+      <c r="L166" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="M166" s="8"/>
       <c r="N166" s="8"/>
       <c r="O166" s="8"/>
@@ -10593,7 +10724,9 @@
       <c r="J167" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="K167" s="8"/>
+      <c r="K167" s="8" t="s">
+        <v>732</v>
+      </c>
       <c r="L167" s="8"/>
       <c r="M167" s="8"/>
       <c r="N167" s="8"/>
@@ -10639,7 +10772,9 @@
       <c r="J168" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="K168" s="8"/>
+      <c r="K168" s="8" t="s">
+        <v>733</v>
+      </c>
       <c r="L168" s="8"/>
       <c r="M168" s="8"/>
       <c r="N168" s="8"/>
@@ -10685,7 +10820,9 @@
       <c r="J169" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="K169" s="8"/>
+      <c r="K169" s="8" t="s">
+        <v>734</v>
+      </c>
       <c r="L169" s="8"/>
       <c r="M169" s="8"/>
       <c r="N169" s="8"/>
@@ -10731,7 +10868,9 @@
       <c r="J170" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="K170" s="8"/>
+      <c r="K170" s="8" t="s">
+        <v>733</v>
+      </c>
       <c r="L170" s="8"/>
       <c r="M170" s="8"/>
       <c r="N170" s="8"/>
@@ -10777,7 +10916,9 @@
       <c r="J171" s="8" t="s">
         <v>708</v>
       </c>
-      <c r="K171" s="8"/>
+      <c r="K171" s="8" t="s">
+        <v>735</v>
+      </c>
       <c r="L171" s="8"/>
       <c r="M171" s="8"/>
       <c r="N171" s="8"/>
@@ -10823,7 +10964,9 @@
       <c r="J172" s="8" t="s">
         <v>712</v>
       </c>
-      <c r="K172" s="8"/>
+      <c r="K172" s="8" t="s">
+        <v>735</v>
+      </c>
       <c r="L172" s="8"/>
       <c r="M172" s="8"/>
       <c r="N172" s="8"/>
@@ -10869,7 +11012,9 @@
       <c r="J173" s="8" t="s">
         <v>716</v>
       </c>
-      <c r="K173" s="8"/>
+      <c r="K173" s="8" t="s">
+        <v>735</v>
+      </c>
       <c r="L173" s="8"/>
       <c r="M173" s="8"/>
       <c r="N173" s="8"/>
@@ -10915,7 +11060,9 @@
       <c r="J174" s="8" t="s">
         <v>719</v>
       </c>
-      <c r="K174" s="8"/>
+      <c r="K174" s="8" t="s">
+        <v>735</v>
+      </c>
       <c r="L174" s="8"/>
       <c r="M174" s="8"/>
       <c r="N174" s="8"/>
@@ -10961,7 +11108,9 @@
       <c r="J175" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="K175" s="8"/>
+      <c r="K175" s="8" t="s">
+        <v>736</v>
+      </c>
       <c r="L175" s="8"/>
       <c r="M175" s="8"/>
       <c r="N175" s="8"/>
@@ -11007,7 +11156,9 @@
       <c r="J176" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="K176" s="8"/>
+      <c r="K176" s="8" t="s">
+        <v>736</v>
+      </c>
       <c r="L176" s="8"/>
       <c r="M176" s="8"/>
       <c r="N176" s="8"/>
@@ -11033,7 +11184,9 @@
       <c r="B177" s="8" t="s">
         <v>729</v>
       </c>
-      <c r="C177" s="8"/>
+      <c r="C177" s="17">
+        <v>43938</v>
+      </c>
       <c r="D177" s="8" t="s">
         <v>20</v>
       </c>
@@ -11051,7 +11204,9 @@
       <c r="J177" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="K177" s="8"/>
+      <c r="K177" s="8" t="s">
+        <v>736</v>
+      </c>
       <c r="L177" s="8"/>
       <c r="M177" s="8"/>
       <c r="N177" s="8"/>
@@ -11070,18 +11225,34 @@
       <c r="AA177" s="6"/>
       <c r="AB177" s="6"/>
     </row>
-    <row r="178" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A178" s="8"/>
-      <c r="B178" s="8"/>
-      <c r="C178" s="8"/>
-      <c r="D178" s="8"/>
+    <row r="178" spans="1:28" ht="51.75" thickBot="1">
+      <c r="A178" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>738</v>
+      </c>
+      <c r="C178" s="17">
+        <v>43941</v>
+      </c>
+      <c r="D178" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E178" s="8"/>
-      <c r="F178" s="8"/>
+      <c r="F178" s="8" t="s">
+        <v>402</v>
+      </c>
       <c r="G178" s="8"/>
-      <c r="H178" s="8"/>
+      <c r="H178" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="I178" s="8"/>
-      <c r="J178" s="8"/>
-      <c r="K178" s="8"/>
+      <c r="J178" s="8" t="s">
+        <v>739</v>
+      </c>
+      <c r="K178" s="8" t="s">
+        <v>740</v>
+      </c>
       <c r="L178" s="8"/>
       <c r="M178" s="8"/>
       <c r="N178" s="8"/>
@@ -11100,18 +11271,34 @@
       <c r="AA178" s="6"/>
       <c r="AB178" s="6"/>
     </row>
-    <row r="179" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A179" s="8"/>
-      <c r="B179" s="8"/>
-      <c r="C179" s="8"/>
-      <c r="D179" s="8"/>
+    <row r="179" spans="1:28" ht="64.5" thickBot="1">
+      <c r="A179" s="8" t="s">
+        <v>741</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>742</v>
+      </c>
+      <c r="C179" s="17">
+        <v>43941</v>
+      </c>
+      <c r="D179" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E179" s="8"/>
-      <c r="F179" s="8"/>
+      <c r="F179" s="8" t="s">
+        <v>301</v>
+      </c>
       <c r="G179" s="8"/>
-      <c r="H179" s="8"/>
+      <c r="H179" s="8" t="s">
+        <v>213</v>
+      </c>
       <c r="I179" s="8"/>
-      <c r="J179" s="8"/>
-      <c r="K179" s="8"/>
+      <c r="J179" s="8" t="s">
+        <v>743</v>
+      </c>
+      <c r="K179" s="8" t="s">
+        <v>377</v>
+      </c>
       <c r="L179" s="8"/>
       <c r="M179" s="8"/>
       <c r="N179" s="8"/>
@@ -11130,18 +11317,34 @@
       <c r="AA179" s="6"/>
       <c r="AB179" s="6"/>
     </row>
-    <row r="180" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A180" s="8"/>
-      <c r="B180" s="8"/>
-      <c r="C180" s="8"/>
-      <c r="D180" s="8"/>
+    <row r="180" spans="1:28" ht="64.5" thickBot="1">
+      <c r="A180" s="8" t="s">
+        <v>744</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>745</v>
+      </c>
+      <c r="C180" s="17">
+        <v>43941</v>
+      </c>
+      <c r="D180" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E180" s="8"/>
-      <c r="F180" s="8"/>
+      <c r="F180" s="8" t="s">
+        <v>301</v>
+      </c>
       <c r="G180" s="8"/>
-      <c r="H180" s="8"/>
+      <c r="H180" s="8" t="s">
+        <v>213</v>
+      </c>
       <c r="I180" s="8"/>
-      <c r="J180" s="8"/>
-      <c r="K180" s="8"/>
+      <c r="J180" s="8" t="s">
+        <v>746</v>
+      </c>
+      <c r="K180" s="8" t="s">
+        <v>377</v>
+      </c>
       <c r="L180" s="8"/>
       <c r="M180" s="8"/>
       <c r="N180" s="8"/>
@@ -11160,18 +11363,34 @@
       <c r="AA180" s="6"/>
       <c r="AB180" s="6"/>
     </row>
-    <row r="181" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A181" s="8"/>
-      <c r="B181" s="8"/>
-      <c r="C181" s="8"/>
-      <c r="D181" s="8"/>
+    <row r="181" spans="1:28" ht="64.5" thickBot="1">
+      <c r="A181" s="8" t="s">
+        <v>747</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>748</v>
+      </c>
+      <c r="C181" s="17">
+        <v>43941</v>
+      </c>
+      <c r="D181" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E181" s="8"/>
-      <c r="F181" s="8"/>
+      <c r="F181" s="8" t="s">
+        <v>301</v>
+      </c>
       <c r="G181" s="8"/>
-      <c r="H181" s="8"/>
+      <c r="H181" s="8" t="s">
+        <v>213</v>
+      </c>
       <c r="I181" s="8"/>
-      <c r="J181" s="8"/>
-      <c r="K181" s="8"/>
+      <c r="J181" s="8" t="s">
+        <v>749</v>
+      </c>
+      <c r="K181" s="8" t="s">
+        <v>377</v>
+      </c>
       <c r="L181" s="8"/>
       <c r="M181" s="8"/>
       <c r="N181" s="8"/>
@@ -11190,19 +11409,31 @@
       <c r="AA181" s="6"/>
       <c r="AB181" s="6"/>
     </row>
-    <row r="182" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A182" s="8"/>
-      <c r="B182" s="8"/>
-      <c r="C182" s="8"/>
-      <c r="D182" s="8"/>
+    <row r="182" spans="1:28" ht="90" thickBot="1">
+      <c r="A182" s="8" t="s">
+        <v>750</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>751</v>
+      </c>
+      <c r="C182" s="17">
+        <v>43941</v>
+      </c>
+      <c r="D182" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E182" s="8"/>
-      <c r="F182" s="8"/>
+      <c r="F182" s="8" t="s">
+        <v>752</v>
+      </c>
       <c r="G182" s="8"/>
       <c r="H182" s="8"/>
       <c r="I182" s="8"/>
       <c r="J182" s="8"/>
       <c r="K182" s="8"/>
-      <c r="L182" s="8"/>
+      <c r="L182" s="8" t="s">
+        <v>367</v>
+      </c>
       <c r="M182" s="8"/>
       <c r="N182" s="8"/>
       <c r="O182" s="8"/>
@@ -11220,19 +11451,31 @@
       <c r="AA182" s="6"/>
       <c r="AB182" s="6"/>
     </row>
-    <row r="183" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A183" s="8"/>
-      <c r="B183" s="8"/>
-      <c r="C183" s="8"/>
-      <c r="D183" s="8"/>
+    <row r="183" spans="1:28" ht="64.5" thickBot="1">
+      <c r="A183" s="8" t="s">
+        <v>753</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>754</v>
+      </c>
+      <c r="C183" s="17">
+        <v>43941</v>
+      </c>
+      <c r="D183" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E183" s="8"/>
-      <c r="F183" s="8"/>
+      <c r="F183" s="8" t="s">
+        <v>755</v>
+      </c>
       <c r="G183" s="8"/>
       <c r="H183" s="8"/>
       <c r="I183" s="8"/>
       <c r="J183" s="8"/>
       <c r="K183" s="8"/>
-      <c r="L183" s="8"/>
+      <c r="L183" s="8" t="s">
+        <v>367</v>
+      </c>
       <c r="M183" s="8"/>
       <c r="N183" s="8"/>
       <c r="O183" s="8"/>
@@ -11250,19 +11493,31 @@
       <c r="AA183" s="6"/>
       <c r="AB183" s="6"/>
     </row>
-    <row r="184" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A184" s="8"/>
-      <c r="B184" s="8"/>
-      <c r="C184" s="8"/>
-      <c r="D184" s="8"/>
+    <row r="184" spans="1:28" ht="51.75" thickBot="1">
+      <c r="A184" s="8" t="s">
+        <v>756</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>757</v>
+      </c>
+      <c r="C184" s="17">
+        <v>43941</v>
+      </c>
+      <c r="D184" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E184" s="8"/>
-      <c r="F184" s="8"/>
+      <c r="F184" s="8" t="s">
+        <v>758</v>
+      </c>
       <c r="G184" s="8"/>
       <c r="H184" s="8"/>
       <c r="I184" s="8"/>
       <c r="J184" s="8"/>
       <c r="K184" s="8"/>
-      <c r="L184" s="8"/>
+      <c r="L184" s="8" t="s">
+        <v>367</v>
+      </c>
       <c r="M184" s="8"/>
       <c r="N184" s="8"/>
       <c r="O184" s="8"/>
@@ -11280,18 +11535,32 @@
       <c r="AA184" s="6"/>
       <c r="AB184" s="6"/>
     </row>
-    <row r="185" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A185" s="8"/>
-      <c r="B185" s="8"/>
-      <c r="C185" s="8"/>
-      <c r="D185" s="8"/>
+    <row r="185" spans="1:28" ht="64.5" thickBot="1">
+      <c r="A185" s="8" t="s">
+        <v>759</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>760</v>
+      </c>
+      <c r="C185" s="17">
+        <v>43942</v>
+      </c>
+      <c r="D185" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E185" s="8"/>
-      <c r="F185" s="8"/>
+      <c r="F185" s="8" t="s">
+        <v>761</v>
+      </c>
       <c r="G185" s="8"/>
-      <c r="H185" s="8"/>
+      <c r="H185" s="8" t="s">
+        <v>762</v>
+      </c>
       <c r="I185" s="8"/>
       <c r="J185" s="8"/>
-      <c r="K185" s="8"/>
+      <c r="K185" s="8" t="s">
+        <v>377</v>
+      </c>
       <c r="L185" s="8"/>
       <c r="M185" s="8"/>
       <c r="N185" s="8"/>
@@ -11310,18 +11579,32 @@
       <c r="AA185" s="6"/>
       <c r="AB185" s="6"/>
     </row>
-    <row r="186" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A186" s="8"/>
-      <c r="B186" s="8"/>
-      <c r="C186" s="8"/>
-      <c r="D186" s="8"/>
+    <row r="186" spans="1:28" ht="64.5" thickBot="1">
+      <c r="A186" s="8" t="s">
+        <v>763</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>760</v>
+      </c>
+      <c r="C186" s="17">
+        <v>43942</v>
+      </c>
+      <c r="D186" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E186" s="8"/>
-      <c r="F186" s="8"/>
+      <c r="F186" s="8" t="s">
+        <v>761</v>
+      </c>
       <c r="G186" s="8"/>
-      <c r="H186" s="8"/>
+      <c r="H186" s="8" t="s">
+        <v>762</v>
+      </c>
       <c r="I186" s="8"/>
       <c r="J186" s="8"/>
-      <c r="K186" s="8"/>
+      <c r="K186" s="8" t="s">
+        <v>312</v>
+      </c>
       <c r="L186" s="8"/>
       <c r="M186" s="8"/>
       <c r="N186" s="8"/>
@@ -11340,18 +11623,32 @@
       <c r="AA186" s="6"/>
       <c r="AB186" s="6"/>
     </row>
-    <row r="187" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A187" s="8"/>
-      <c r="B187" s="8"/>
-      <c r="C187" s="8"/>
-      <c r="D187" s="8"/>
+    <row r="187" spans="1:28" ht="64.5" thickBot="1">
+      <c r="A187" s="8" t="s">
+        <v>764</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>765</v>
+      </c>
+      <c r="C187" s="17">
+        <v>43942</v>
+      </c>
+      <c r="D187" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E187" s="8"/>
-      <c r="F187" s="8"/>
+      <c r="F187" s="8" t="s">
+        <v>761</v>
+      </c>
       <c r="G187" s="8"/>
-      <c r="H187" s="8"/>
+      <c r="H187" s="8" t="s">
+        <v>762</v>
+      </c>
       <c r="I187" s="8"/>
       <c r="J187" s="8"/>
-      <c r="K187" s="8"/>
+      <c r="K187" s="8" t="s">
+        <v>377</v>
+      </c>
       <c r="L187" s="8"/>
       <c r="M187" s="8"/>
       <c r="N187" s="8"/>
@@ -11370,18 +11667,32 @@
       <c r="AA187" s="6"/>
       <c r="AB187" s="6"/>
     </row>
-    <row r="188" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A188" s="8"/>
-      <c r="B188" s="8"/>
-      <c r="C188" s="8"/>
-      <c r="D188" s="8"/>
+    <row r="188" spans="1:28" ht="64.5" thickBot="1">
+      <c r="A188" s="8" t="s">
+        <v>766</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>767</v>
+      </c>
+      <c r="C188" s="17">
+        <v>43942</v>
+      </c>
+      <c r="D188" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E188" s="8"/>
-      <c r="F188" s="8"/>
+      <c r="F188" s="8" t="s">
+        <v>761</v>
+      </c>
       <c r="G188" s="8"/>
-      <c r="H188" s="8"/>
+      <c r="H188" s="8" t="s">
+        <v>762</v>
+      </c>
       <c r="I188" s="8"/>
       <c r="J188" s="8"/>
-      <c r="K188" s="8"/>
+      <c r="K188" s="8" t="s">
+        <v>377</v>
+      </c>
       <c r="L188" s="8"/>
       <c r="M188" s="8"/>
       <c r="N188" s="8"/>
@@ -11400,18 +11711,32 @@
       <c r="AA188" s="6"/>
       <c r="AB188" s="6"/>
     </row>
-    <row r="189" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A189" s="8"/>
-      <c r="B189" s="8"/>
-      <c r="C189" s="8"/>
-      <c r="D189" s="8"/>
+    <row r="189" spans="1:28" ht="39" thickBot="1">
+      <c r="A189" s="8" t="s">
+        <v>768</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="C189" s="17">
+        <v>43942</v>
+      </c>
+      <c r="D189" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E189" s="8"/>
-      <c r="F189" s="8"/>
+      <c r="F189" s="8" t="s">
+        <v>402</v>
+      </c>
       <c r="G189" s="8"/>
-      <c r="H189" s="8"/>
+      <c r="H189" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="I189" s="8"/>
       <c r="J189" s="8"/>
-      <c r="K189" s="8"/>
+      <c r="K189" s="8" t="s">
+        <v>769</v>
+      </c>
       <c r="L189" s="8"/>
       <c r="M189" s="8"/>
       <c r="N189" s="8"/>
@@ -11430,18 +11755,32 @@
       <c r="AA189" s="6"/>
       <c r="AB189" s="6"/>
     </row>
-    <row r="190" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A190" s="8"/>
-      <c r="B190" s="8"/>
-      <c r="C190" s="8"/>
-      <c r="D190" s="8"/>
+    <row r="190" spans="1:28" ht="51.75" thickBot="1">
+      <c r="A190" s="8" t="s">
+        <v>770</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>771</v>
+      </c>
+      <c r="C190" s="17">
+        <v>43943</v>
+      </c>
+      <c r="D190" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E190" s="8"/>
-      <c r="F190" s="8"/>
+      <c r="F190" s="8" t="s">
+        <v>367</v>
+      </c>
       <c r="G190" s="8"/>
-      <c r="H190" s="8"/>
+      <c r="H190" s="8" t="s">
+        <v>694</v>
+      </c>
       <c r="I190" s="8"/>
       <c r="J190" s="8"/>
-      <c r="K190" s="8"/>
+      <c r="K190" s="8" t="s">
+        <v>772</v>
+      </c>
       <c r="L190" s="8"/>
       <c r="M190" s="8"/>
       <c r="N190" s="8"/>
@@ -11460,18 +11799,32 @@
       <c r="AA190" s="6"/>
       <c r="AB190" s="6"/>
     </row>
-    <row r="191" spans="1:28" ht="16.5" thickBot="1">
-      <c r="A191" s="8"/>
-      <c r="B191" s="8"/>
-      <c r="C191" s="8"/>
-      <c r="D191" s="8"/>
+    <row r="191" spans="1:28" ht="51.75" thickBot="1">
+      <c r="A191" s="8" t="s">
+        <v>773</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>774</v>
+      </c>
+      <c r="C191" s="17">
+        <v>43943</v>
+      </c>
+      <c r="D191" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="E191" s="8"/>
-      <c r="F191" s="8"/>
+      <c r="F191" s="8" t="s">
+        <v>367</v>
+      </c>
       <c r="G191" s="8"/>
-      <c r="H191" s="8"/>
+      <c r="H191" s="8" t="s">
+        <v>694</v>
+      </c>
       <c r="I191" s="8"/>
       <c r="J191" s="8"/>
-      <c r="K191" s="8"/>
+      <c r="K191" s="8" t="s">
+        <v>769</v>
+      </c>
       <c r="L191" s="8"/>
       <c r="M191" s="8"/>
       <c r="N191" s="8"/>

</xml_diff>